<commit_message>
Update Backtest Results v1.1.xlsx
</commit_message>
<xml_diff>
--- a/Strategies/Box Breakout/Backtesting/Backtest Results v1.1.xlsx
+++ b/Strategies/Box Breakout/Backtesting/Backtest Results v1.1.xlsx
@@ -5,20 +5,23 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerry\AppData\Roaming\MetaQuotes\Terminal\D0E8209F77C8CF37AD8BF550E51FF075\MQL5\Experts\Forex-Algotrading-Strategies--MQL5-\Strategies\Box Breakout\Pairs\USDJPY\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerry\AppData\Roaming\MetaQuotes\Terminal\D0E8209F77C8CF37AD8BF550E51FF075\MQL5\Experts\Forex-Algotrading-Strategies--MQL5-\Strategies\Box Breakout\Backtesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD921730-15D9-48D1-91AF-06CCA1DFDFE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6549E14D-4A15-45E5-9B20-A87B71C9349C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{A4C4D3AB-FFA6-4A76-82A7-BA4091383E73}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{A4C4D3AB-FFA6-4A76-82A7-BA4091383E73}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison" sheetId="2" r:id="rId1"/>
     <sheet name="UJ-5Y --&gt;" sheetId="5" r:id="rId2"/>
-    <sheet name="TPF2-TSL-NoTnd-R2" sheetId="7" r:id="rId3"/>
-    <sheet name="TPF2-TSL-NoTnd-R1" sheetId="6" r:id="rId4"/>
+    <sheet name="NoTP-TSL-Tnd-R1" sheetId="11" r:id="rId3"/>
+    <sheet name="TPF2.5-TSL-Tnd-R1" sheetId="1" r:id="rId4"/>
     <sheet name="TPF2-TSL-Tnd-R1" sheetId="4" r:id="rId5"/>
-    <sheet name="TPF2.5-TSL-Tnd-R1" sheetId="1" r:id="rId6"/>
+    <sheet name="NoTP-NoTSL-NoTnd-R1" sheetId="10" r:id="rId6"/>
+    <sheet name="TPF2-TSL-NoTnd-R1" sheetId="6" r:id="rId7"/>
+    <sheet name="NoTP-NoTSL-NoTnd-R2" sheetId="9" r:id="rId8"/>
+    <sheet name="TPF2-TSL-NoTnd-R2" sheetId="7" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="69">
   <si>
     <t>Inputs</t>
   </si>
@@ -180,16 +183,83 @@
   </si>
   <si>
     <t>TPF2-TSL-NoTnd-R2</t>
+  </si>
+  <si>
+    <t>NoTP-TSL-NoTnd-R2</t>
+  </si>
+  <si>
+    <t>NoTP-TSL-Tnd-R1</t>
+  </si>
+  <si>
+    <t>How to read test codes</t>
+  </si>
+  <si>
+    <t>[Trailing Stop Loss]</t>
+  </si>
+  <si>
+    <t>[Trend]</t>
+  </si>
+  <si>
+    <t>[Range]</t>
+  </si>
+  <si>
+    <t>[Take Profit]</t>
+  </si>
+  <si>
+    <t>NoTP = No Take Profit</t>
+  </si>
+  <si>
+    <t>TPF2.5 = Take Profit Factor of 2.5</t>
+  </si>
+  <si>
+    <t>TPF2 = Take Profit Factor of 2</t>
+  </si>
+  <si>
+    <t>NoTP-NoTSL-NoTnd-R1</t>
+  </si>
+  <si>
+    <t>NoTSL = No Trailing Stop Loss</t>
+  </si>
+  <si>
+    <t>TSL = Trailing Stop Loss</t>
+  </si>
+  <si>
+    <t>Tnd = Force Trades to Follow Trend</t>
+  </si>
+  <si>
+    <t>Tnd = Don't Force Trades to Follow Trend</t>
+  </si>
+  <si>
+    <t>R1 = Range Settings 1</t>
+  </si>
+  <si>
+    <t>R2 = Range Settings 2</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Taking this to FTMO to trade</t>
+  </si>
+  <si>
+    <t>Profit Factor</t>
+  </si>
+  <si>
+    <t>Range 2 is is not it…</t>
+  </si>
+  <si>
+    <t>Way overleveraged</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -216,6 +286,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -255,7 +331,7 @@
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -269,13 +345,37 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -293,13 +393,835 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>173277</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>743</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A7D4E88-CBC0-86FF-8708-12D0E8AA2E24}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4057650" y="1228725"/>
+          <a:ext cx="13089177" cy="5325218"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>449490</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>114824</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B7BBA598-9048-C84E-1579-2B773570DA84}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4419600" y="6915150"/>
+          <a:ext cx="13003440" cy="3753374"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>420895</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>133891</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE65BA8D-F40F-04AB-3527-B724E7DCC87F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4533900" y="10810875"/>
+          <a:ext cx="12860545" cy="3877216"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>392338</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>528</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE390BD3-5765-EEE6-FA24-681E9357FF14}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3276600" y="1438275"/>
+          <a:ext cx="12993913" cy="3781953"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>468524</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>162416</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{86D31858-587E-37FF-3553-283F89E400B0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3457575" y="5295900"/>
+          <a:ext cx="12889124" cy="3515216"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>344683</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>57646</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4FE0A5DB-7C19-C39D-9171-62B2AFFB2E9E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3562350" y="8963025"/>
+          <a:ext cx="12774808" cy="3553321"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>487596</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>10034</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D122609-6CB2-74AC-F923-B9D8067CE89B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4410075" y="5391150"/>
+          <a:ext cx="13051071" cy="3648584"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>287559</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>48155</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B0A462D6-5344-9BDB-38A4-3EE428108B51}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4295775" y="1466850"/>
+          <a:ext cx="12965334" cy="3801005"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>478042</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>57657</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38DEB879-A7D9-D581-C7DC-3C0A6AB80EF6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4610100" y="9077325"/>
+          <a:ext cx="12841492" cy="3629532"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>116103</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>86238</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{127ADE2A-7514-8CA5-17FA-14C5AA7A7099}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4171950" y="6581775"/>
+          <a:ext cx="12917703" cy="3677163"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>154192</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>10004</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2882D67-4D81-DC71-4B30-F2DEC5B0B0B9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4286250" y="10182225"/>
+          <a:ext cx="12841492" cy="3429479"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>66642</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>164145</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4085C65F-738E-A5E2-CA90-C5FD3DE73E97}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4324350" y="1095342"/>
+          <a:ext cx="12820650" cy="5431503"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>306615</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>124361</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{77A2F8B0-6060-6DFA-D03E-43C803BBA367}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4286250" y="5314950"/>
+          <a:ext cx="13003440" cy="3839111"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>211361</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>152918</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62B593A8-EBB3-4108-9D2A-E66C9894514C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4219575" y="1466850"/>
+          <a:ext cx="12974861" cy="3715268"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>230388</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>86212</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5AC73D90-BF59-62EB-B395-349F964BED85}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4400550" y="9248775"/>
+          <a:ext cx="12812913" cy="3486637"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>459012</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>171988</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92D71DD8-AA92-D1BF-A2CE-8885D0B09085}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4448175" y="1343025"/>
+          <a:ext cx="12984387" cy="3858163"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>468538</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>171986</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E180EA5-27EA-03C0-0F64-44B24FF9D82D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4448175" y="5172075"/>
+          <a:ext cx="12993913" cy="3839111"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>373264</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>114858</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B0CD63D1-D54F-F5A3-CE91-1490777BB4E2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4524375" y="9144000"/>
+          <a:ext cx="12822439" cy="4001058"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>390525</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>563784</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>382809</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>181509</xdr:rowOff>
     </xdr:to>
@@ -342,8 +1264,8 @@
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>544729</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>363754</xdr:colOff>
       <xdr:row>48</xdr:row>
       <xdr:rowOff>10067</xdr:rowOff>
     </xdr:to>
@@ -386,8 +1308,8 @@
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>592362</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>411387</xdr:colOff>
       <xdr:row>67</xdr:row>
       <xdr:rowOff>76692</xdr:rowOff>
     </xdr:to>
@@ -414,417 +1336,6 @@
         <a:xfrm>
           <a:off x="4400550" y="9391650"/>
           <a:ext cx="12984387" cy="3524742"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>497115</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>124361</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{77A2F8B0-6060-6DFA-D03E-43C803BBA367}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4286250" y="5314950"/>
-          <a:ext cx="13003440" cy="3839111"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>401861</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>152918</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62B593A8-EBB3-4108-9D2A-E66C9894514C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4219575" y="1466850"/>
-          <a:ext cx="12974861" cy="3715268"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>420888</xdr:colOff>
-      <xdr:row>66</xdr:row>
-      <xdr:rowOff>86212</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Picture 6">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5AC73D90-BF59-62EB-B395-349F964BED85}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4400550" y="9248775"/>
-          <a:ext cx="12812913" cy="3486637"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>58971</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>10034</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D122609-6CB2-74AC-F923-B9D8067CE89B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4410075" y="5391150"/>
-          <a:ext cx="13051071" cy="3648584"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>468534</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>48155</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B0A462D6-5344-9BDB-38A4-3EE428108B51}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4295775" y="1466850"/>
-          <a:ext cx="12965334" cy="3801005"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>49417</xdr:colOff>
-      <xdr:row>66</xdr:row>
-      <xdr:rowOff>57657</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Picture 6">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38DEB879-A7D9-D581-C7DC-3C0A6AB80EF6}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4610100" y="9077325"/>
-          <a:ext cx="12841492" cy="3629532"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>573313</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>528</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE390BD3-5765-EEE6-FA24-681E9357FF14}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3276600" y="1438275"/>
-          <a:ext cx="12993913" cy="3781953"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>39899</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>162416</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{86D31858-587E-37FF-3553-283F89E400B0}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3457575" y="5295900"/>
-          <a:ext cx="12889124" cy="3515216"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>525658</xdr:colOff>
-      <xdr:row>64</xdr:row>
-      <xdr:rowOff>57646</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4FE0A5DB-7C19-C39D-9171-62B2AFFB2E9E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3562350" y="8963025"/>
-          <a:ext cx="12774808" cy="3553321"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1133,208 +1644,455 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1272344-E85B-4763-A4E4-CD05299D91FF}">
-  <dimension ref="B2:I13"/>
+  <dimension ref="B2:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T14" sqref="T14"/>
+      <selection activeCell="C18" sqref="C18:K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" customWidth="1"/>
-    <col min="6" max="6" width="20.42578125" customWidth="1"/>
-    <col min="7" max="7" width="18.7109375" customWidth="1"/>
-    <col min="8" max="8" width="14.85546875" customWidth="1"/>
-    <col min="9" max="9" width="16" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" customWidth="1"/>
+    <col min="4" max="4" width="38.5703125" customWidth="1"/>
+    <col min="5" max="6" width="23.140625" customWidth="1"/>
+    <col min="7" max="7" width="20.42578125" customWidth="1"/>
+    <col min="8" max="8" width="18.7109375" customWidth="1"/>
+    <col min="9" max="9" width="14.85546875" customWidth="1"/>
+    <col min="10" max="10" width="16" customWidth="1"/>
+    <col min="11" max="11" width="27.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C14" s="11">
         <v>10000</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="3" t="s">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C15" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D15" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E15" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F15" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="H15" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="I15" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="J15" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+      <c r="K15" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
         <v>42</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" s="6">
+        <f>'NoTP-TSL-Tnd-R1'!F4</f>
+        <v>17450.39</v>
+      </c>
+      <c r="E16" s="10">
+        <f>'NoTP-TSL-Tnd-R1'!G4</f>
+        <v>1.745039</v>
+      </c>
+      <c r="F16" s="13">
+        <f>'NoTP-TSL-Tnd-R1'!H4</f>
+        <v>1.51</v>
+      </c>
+      <c r="G16" s="7">
+        <f>'NoTP-TSL-Tnd-R1'!I4</f>
+        <v>2271.67</v>
+      </c>
+      <c r="H16" s="10">
+        <f>'NoTP-TSL-Tnd-R1'!J4</f>
+        <v>8.7499999999999994E-2</v>
+      </c>
+      <c r="I16" s="10">
+        <f>'NoTP-TSL-Tnd-R1'!K4</f>
+        <v>0.61760000000000004</v>
+      </c>
+      <c r="J16">
+        <f>'NoTP-TSL-Tnd-R1'!L4</f>
+        <v>918</v>
+      </c>
+      <c r="K16" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" s="7">
+        <f>'TPF2-TSL-Tnd-R1'!F4</f>
+        <v>13537.36</v>
+      </c>
+      <c r="E17" s="10">
+        <f>'TPF2-TSL-Tnd-R1'!G5</f>
+        <v>1.3537360000000001</v>
+      </c>
+      <c r="F17" s="13">
+        <f>'TPF2-TSL-Tnd-R1'!H5</f>
+        <v>1.41</v>
+      </c>
+      <c r="G17" s="7">
+        <f>'TPF2-TSL-Tnd-R1'!I4</f>
+        <v>2098.73</v>
+      </c>
+      <c r="H17" s="10">
+        <f>'TPF2-TSL-Tnd-R1'!J4</f>
+        <v>9.0200000000000002E-2</v>
+      </c>
+      <c r="I17" s="10">
+        <f>'TPF2-TSL-Tnd-R1'!K4</f>
+        <v>0.3856</v>
+      </c>
+      <c r="J17">
+        <f>'TPF2-TSL-Tnd-R1'!L4</f>
+        <v>918</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D18" s="6">
         <f>'TPF2.5-TSL-Tnd-R1'!F4</f>
         <v>11320.79</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E18" s="10">
         <f>'TPF2.5-TSL-Tnd-R1'!G4</f>
         <v>1.1320790000000001</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F18" s="13">
         <f>'TPF2.5-TSL-Tnd-R1'!H4</f>
+        <v>1.38</v>
+      </c>
+      <c r="G18" s="7">
+        <f>'TPF2.5-TSL-Tnd-R1'!I4</f>
         <v>2181.52</v>
       </c>
-      <c r="G10" s="10">
-        <f>'TPF2.5-TSL-Tnd-R1'!I4</f>
+      <c r="H18" s="10">
+        <f>'TPF2.5-TSL-Tnd-R1'!J4</f>
         <v>0.1043</v>
       </c>
-      <c r="H10" s="10">
-        <f>'TPF2.5-TSL-Tnd-R1'!J4</f>
+      <c r="I18" s="10">
+        <f>'TPF2.5-TSL-Tnd-R1'!K4</f>
         <v>0.61760000000000004</v>
       </c>
-      <c r="I10">
-        <f>'TPF2.5-TSL-Tnd-R1'!K4</f>
+      <c r="J18">
+        <f>'TPF2.5-TSL-Tnd-R1'!L4</f>
         <v>918</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
         <v>42</v>
       </c>
-      <c r="C11" t="s">
-        <v>44</v>
-      </c>
-      <c r="D11" s="7">
-        <f>'TPF2-TSL-Tnd-R1'!F4</f>
-        <v>13537.36</v>
-      </c>
-      <c r="E11" s="10">
-        <f>'TPF2-TSL-Tnd-R1'!G5</f>
-        <v>1.3537360000000001</v>
-      </c>
-      <c r="F11" s="7">
-        <f>'TPF2-TSL-Tnd-R1'!H4</f>
-        <v>2181.52</v>
-      </c>
-      <c r="G11" s="10">
-        <f>'TPF2-TSL-Tnd-R1'!I4</f>
-        <v>9.0200000000000002E-2</v>
-      </c>
-      <c r="H11" s="10">
-        <f>'TPF2-TSL-Tnd-R1'!J4</f>
-        <v>0.3856</v>
-      </c>
-      <c r="I11">
-        <f>'TPF2-TSL-Tnd-R1'!K4</f>
-        <v>918</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>42</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="C19" t="s">
         <v>45</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D19" s="7">
         <f>'TPF2-TSL-NoTnd-R1'!F4</f>
         <v>14904.36</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E19" s="10">
         <f>'TPF2-TSL-NoTnd-R1'!G4</f>
         <v>1.4904360000000001</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F19" s="13">
         <f>'TPF2-TSL-NoTnd-R1'!H4</f>
+        <v>1.21</v>
+      </c>
+      <c r="G19" s="7">
+        <f>'TPF2-TSL-NoTnd-R1'!I4</f>
         <v>3601.63</v>
       </c>
-      <c r="G12" s="10">
-        <f>'TPF2-TSL-NoTnd-R1'!I5</f>
+      <c r="H19" s="10">
+        <f>'TPF2-TSL-NoTnd-R1'!J5</f>
         <v>0.13289999999999999</v>
       </c>
-      <c r="H12" s="10">
-        <f>'TPF2-TSL-NoTnd-R1'!J4</f>
+      <c r="I19" s="10">
+        <f>'TPF2-TSL-NoTnd-R1'!K4</f>
         <v>0.36</v>
       </c>
-      <c r="I12">
-        <f>'TPF2-TSL-NoTnd-R1'!K4</f>
+      <c r="J19">
+        <f>'TPF2-TSL-NoTnd-R1'!L4</f>
         <v>1747</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
         <v>42</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C20" t="s">
         <v>46</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D20" s="7">
         <f>'TPF2-TSL-NoTnd-R2'!F4</f>
         <v>10926.29</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E20" s="10">
         <f>'TPF2-TSL-NoTnd-R2'!G4</f>
         <v>1.0926290000000001</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F20" s="13">
         <f>'TPF2-TSL-NoTnd-R2'!H4</f>
+        <v>1.21</v>
+      </c>
+      <c r="G20" s="7">
+        <f>'TPF2-TSL-NoTnd-R2'!I4</f>
         <v>2566.5300000000002</v>
       </c>
-      <c r="G13" s="10">
-        <f>'TPF2-TSL-NoTnd-R2'!I4</f>
+      <c r="H20" s="10">
+        <f>'TPF2-TSL-NoTnd-R2'!J4</f>
         <v>0.1178</v>
       </c>
-      <c r="H13" s="10">
-        <f>'TPF2-TSL-NoTnd-R2'!J4</f>
+      <c r="I20" s="10">
+        <f>'TPF2-TSL-NoTnd-R2'!K4</f>
         <v>0.3518</v>
       </c>
-      <c r="I13">
-        <f>'TPF2-TSL-NoTnd-R2'!K4</f>
+      <c r="J20">
+        <f>'TPF2-TSL-NoTnd-R2'!L4</f>
         <v>1444</v>
       </c>
+      <c r="K20" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" t="s">
+        <v>57</v>
+      </c>
+      <c r="D21" s="7">
+        <f>'NoTP-NoTSL-NoTnd-R1'!F4</f>
+        <v>23386.57</v>
+      </c>
+      <c r="E21" s="10">
+        <f>'NoTP-NoTSL-NoTnd-R1'!G4</f>
+        <v>2.338657</v>
+      </c>
+      <c r="F21" s="13">
+        <f>'NoTP-NoTSL-NoTnd-R1'!H4</f>
+        <v>1.2</v>
+      </c>
+      <c r="G21" s="7">
+        <f>'NoTP-NoTSL-NoTnd-R1'!I4</f>
+        <v>6243.47</v>
+      </c>
+      <c r="H21" s="10">
+        <f>'NoTP-NoTSL-NoTnd-R1'!J4</f>
+        <v>0.17249999999999999</v>
+      </c>
+      <c r="I21" s="10">
+        <f>'NoTP-NoTSL-NoTnd-R1'!K4</f>
+        <v>0.435</v>
+      </c>
+      <c r="J21">
+        <f>'NoTP-NoTSL-NoTnd-R1'!L4</f>
+        <v>1747</v>
+      </c>
+      <c r="K21" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" t="s">
+        <v>47</v>
+      </c>
+      <c r="D22" s="7">
+        <f>'NoTP-NoTSL-NoTnd-R2'!F4</f>
+        <v>14234.069999999998</v>
+      </c>
+      <c r="E22" s="10">
+        <f>'NoTP-NoTSL-NoTnd-R2'!G4</f>
+        <v>1.4234069999999999</v>
+      </c>
+      <c r="F22" s="13">
+        <f>'NoTP-NoTSL-NoTnd-R2'!H4</f>
+        <v>1.18</v>
+      </c>
+      <c r="G22" s="7">
+        <f>'NoTP-NoTSL-NoTnd-R2'!I4</f>
+        <v>3787.72</v>
+      </c>
+      <c r="H22" s="10">
+        <f>'NoTP-NoTSL-NoTnd-R2'!J4</f>
+        <v>0.14849999999999999</v>
+      </c>
+      <c r="I22" s="10">
+        <f>'NoTP-NoTSL-NoTnd-R2'!K4</f>
+        <v>0.42799999999999999</v>
+      </c>
+      <c r="J22">
+        <f>'NoTP-NoTSL-NoTnd-R2'!L4</f>
+        <v>1444</v>
+      </c>
+      <c r="K22" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D23" s="7"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <conditionalFormatting sqref="H16:H22">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="lessThan">
+      <formula>0.1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="5" operator="greaterThan">
+      <formula>0.1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D16:D22">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E16:F22">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G16:G22">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1357,11 +2115,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01C3B81C-4620-4EB9-8F0B-B8F5A41B29BF}">
-  <dimension ref="A1:K28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{255B4DC5-8A1E-44E0-8BED-166F30CBAE4B}">
+  <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1370,22 +2128,23 @@
     <col min="4" max="4" width="16.42578125" customWidth="1"/>
     <col min="5" max="5" width="16.5703125" customWidth="1"/>
     <col min="6" max="6" width="21.42578125" customWidth="1"/>
-    <col min="7" max="7" width="21" customWidth="1"/>
-    <col min="8" max="8" width="22.7109375" customWidth="1"/>
-    <col min="9" max="9" width="18.85546875" customWidth="1"/>
-    <col min="10" max="10" width="15.85546875" customWidth="1"/>
-    <col min="11" max="11" width="20.5703125" customWidth="1"/>
+    <col min="7" max="8" width="21" customWidth="1"/>
+    <col min="9" max="9" width="22.7109375" customWidth="1"/>
+    <col min="10" max="10" width="18.85546875" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" customWidth="1"/>
+    <col min="12" max="12" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G2" s="6"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H2" s="6"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -1397,19 +2156,22 @@
         <v>23</v>
       </c>
       <c r="H3" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="K3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="L3" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1420,35 +2182,39 @@
         <v>40</v>
       </c>
       <c r="E4" s="6">
-        <f>Comparison!C8</f>
+        <f>Comparison!C14</f>
         <v>10000</v>
       </c>
       <c r="F4" s="7">
         <f>E4*(F5/10000)</f>
-        <v>10926.29</v>
+        <v>17450.39</v>
       </c>
       <c r="G4" s="9">
         <f>F4/E4</f>
-        <v>1.0926290000000001</v>
-      </c>
-      <c r="H4" s="7">
-        <f>E4*(H5/10000)</f>
-        <v>2566.5300000000002</v>
-      </c>
-      <c r="I4" s="9">
-        <f>I5</f>
-        <v>0.1178</v>
+        <v>1.745039</v>
+      </c>
+      <c r="H4" s="12">
+        <f>H5</f>
+        <v>1.51</v>
+      </c>
+      <c r="I4" s="7">
+        <f>E4*(I5/10000)</f>
+        <v>2271.67</v>
       </c>
       <c r="J4" s="9">
         <f>J5</f>
-        <v>0.3518</v>
-      </c>
-      <c r="K4" s="8">
+        <v>8.7499999999999994E-2</v>
+      </c>
+      <c r="K4" s="9">
         <f>K5</f>
-        <v>1444</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+        <v>0.61760000000000004</v>
+      </c>
+      <c r="L4" s="8">
+        <f>L5</f>
+        <v>918</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1459,26 +2225,29 @@
         <v>10000</v>
       </c>
       <c r="F5" s="6">
-        <v>10926.29</v>
+        <v>17450.39</v>
       </c>
       <c r="G5" s="9">
         <f>F5/E5</f>
-        <v>1.0926290000000001</v>
-      </c>
-      <c r="H5" s="6">
-        <v>2566.5300000000002</v>
-      </c>
-      <c r="I5" s="9">
-        <v>0.1178</v>
+        <v>1.745039</v>
+      </c>
+      <c r="H5" s="12">
+        <v>1.51</v>
+      </c>
+      <c r="I5" s="6">
+        <v>2271.67</v>
       </c>
       <c r="J5" s="9">
-        <v>0.3518</v>
-      </c>
-      <c r="K5" s="8">
-        <v>1444</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+        <v>8.7499999999999994E-2</v>
+      </c>
+      <c r="K5" s="9">
+        <v>0.61760000000000004</v>
+      </c>
+      <c r="L5" s="8">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1486,21 +2255,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="4"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1508,7 +2277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1516,29 +2285,29 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B12" s="4"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>37</v>
       </c>
       <c r="B13" s="5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -1546,7 +2315,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -1554,7 +2323,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -1664,11 +2433,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6782CC76-D1C3-4963-AF90-AA17344F07D5}">
-  <dimension ref="A1:K28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66E18A51-5F60-4412-BADD-DCCB6661D68E}">
+  <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="X21" sqref="X21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1677,22 +2446,23 @@
     <col min="4" max="4" width="16.42578125" customWidth="1"/>
     <col min="5" max="5" width="16.5703125" customWidth="1"/>
     <col min="6" max="6" width="21.42578125" customWidth="1"/>
-    <col min="7" max="7" width="21" customWidth="1"/>
-    <col min="8" max="8" width="22.7109375" customWidth="1"/>
-    <col min="9" max="9" width="18.85546875" customWidth="1"/>
-    <col min="10" max="10" width="15.85546875" customWidth="1"/>
-    <col min="11" max="11" width="20.5703125" customWidth="1"/>
+    <col min="7" max="8" width="21" customWidth="1"/>
+    <col min="9" max="9" width="22.7109375" customWidth="1"/>
+    <col min="10" max="10" width="18.85546875" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" customWidth="1"/>
+    <col min="12" max="12" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G2" s="6"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H2" s="6"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -1704,19 +2474,22 @@
         <v>23</v>
       </c>
       <c r="H3" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="K3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="L3" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1727,35 +2500,36 @@
         <v>40</v>
       </c>
       <c r="E4" s="6">
-        <f>Comparison!C8</f>
+        <f>Comparison!C14</f>
         <v>10000</v>
       </c>
       <c r="F4" s="7">
         <f>E4*(F5/10000)</f>
-        <v>14904.36</v>
+        <v>11320.79</v>
       </c>
       <c r="G4" s="9">
         <f>F4/E4</f>
-        <v>1.4904360000000001</v>
-      </c>
-      <c r="H4" s="7">
-        <f>E4*(H5/10000)</f>
-        <v>3601.63</v>
-      </c>
-      <c r="I4" s="9">
-        <f>I5</f>
-        <v>0.13289999999999999</v>
+        <v>1.1320790000000001</v>
+      </c>
+      <c r="H4" s="12">
+        <f>H5</f>
+        <v>1.38</v>
+      </c>
+      <c r="I4" s="7">
+        <f>E4*(I5/10000)</f>
+        <v>2181.52</v>
       </c>
       <c r="J4" s="9">
-        <f>J5</f>
-        <v>0.36</v>
-      </c>
-      <c r="K4" s="8">
-        <f>K5</f>
-        <v>1747</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+        <v>0.1043</v>
+      </c>
+      <c r="K4" s="9">
+        <v>0.61760000000000004</v>
+      </c>
+      <c r="L4" s="8">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1766,26 +2540,30 @@
         <v>10000</v>
       </c>
       <c r="F5" s="6">
-        <v>14904.36</v>
+        <v>11320.79</v>
       </c>
       <c r="G5" s="9">
         <f>F5/E5</f>
-        <v>1.4904360000000001</v>
-      </c>
-      <c r="H5" s="6">
-        <v>3601.63</v>
-      </c>
-      <c r="I5" s="9">
-        <v>0.13289999999999999</v>
+        <v>1.1320790000000001</v>
+      </c>
+      <c r="H5" s="12">
+        <v>1.38</v>
+      </c>
+      <c r="I5" s="6">
+        <f>2181.52</f>
+        <v>2181.52</v>
       </c>
       <c r="J5" s="9">
-        <v>0.36</v>
-      </c>
-      <c r="K5" s="8">
-        <v>1747</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+        <v>0.1043</v>
+      </c>
+      <c r="K5" s="9">
+        <v>0.61760000000000004</v>
+      </c>
+      <c r="L5" s="8">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1793,21 +2571,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="4"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1815,7 +2593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1823,29 +2601,29 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B12" s="4"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>37</v>
       </c>
       <c r="B13" s="5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -1853,7 +2631,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -1861,7 +2639,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -1972,10 +2750,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7319F233-2FAA-4C26-94A4-42EAB123CA4A}">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E53" sqref="E53"/>
+      <selection activeCell="H2" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1984,22 +2762,23 @@
     <col min="4" max="4" width="16.42578125" customWidth="1"/>
     <col min="5" max="5" width="16.5703125" customWidth="1"/>
     <col min="6" max="6" width="21.42578125" customWidth="1"/>
-    <col min="7" max="7" width="21" customWidth="1"/>
-    <col min="8" max="8" width="22.7109375" customWidth="1"/>
-    <col min="9" max="9" width="18.85546875" customWidth="1"/>
-    <col min="10" max="10" width="15.85546875" customWidth="1"/>
-    <col min="11" max="11" width="20.5703125" customWidth="1"/>
+    <col min="7" max="8" width="21" customWidth="1"/>
+    <col min="9" max="9" width="22.7109375" customWidth="1"/>
+    <col min="10" max="10" width="18.85546875" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" customWidth="1"/>
+    <col min="12" max="12" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G2" s="6"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H2" s="6"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -2011,19 +2790,22 @@
         <v>23</v>
       </c>
       <c r="H3" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="K3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="L3" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -2034,7 +2816,7 @@
         <v>40</v>
       </c>
       <c r="E4" s="6">
-        <f>Comparison!C8</f>
+        <f>Comparison!C14</f>
         <v>10000</v>
       </c>
       <c r="F4" s="7">
@@ -2045,24 +2827,28 @@
         <f>F4/E4</f>
         <v>1.3537360000000001</v>
       </c>
-      <c r="H4" s="7">
-        <f>E4*(H5/10000)</f>
-        <v>2181.52</v>
-      </c>
-      <c r="I4" s="9">
-        <f>I5</f>
-        <v>9.0200000000000002E-2</v>
+      <c r="H4" s="12">
+        <f>H5</f>
+        <v>1.41</v>
+      </c>
+      <c r="I4" s="7">
+        <f>E4*(I5/10000)</f>
+        <v>2098.73</v>
       </c>
       <c r="J4" s="9">
         <f>J5</f>
+        <v>9.0200000000000002E-2</v>
+      </c>
+      <c r="K4" s="9">
+        <f>K5</f>
         <v>0.3856</v>
       </c>
-      <c r="K4" s="8">
-        <f>K5</f>
+      <c r="L4" s="8">
+        <f>L5</f>
         <v>918</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -2079,21 +2865,23 @@
         <f>F5/E5</f>
         <v>1.3537360000000001</v>
       </c>
-      <c r="H5" s="6">
-        <f>2181.52</f>
-        <v>2181.52</v>
-      </c>
-      <c r="I5" s="9">
+      <c r="H5" s="12">
+        <v>1.41</v>
+      </c>
+      <c r="I5" s="6">
+        <v>2098.73</v>
+      </c>
+      <c r="J5" s="9">
         <v>9.0200000000000002E-2</v>
       </c>
-      <c r="J5" s="9">
+      <c r="K5" s="9">
         <v>0.3856</v>
       </c>
-      <c r="K5" s="8">
+      <c r="L5" s="8">
         <v>918</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -2101,7 +2889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -2109,13 +2897,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="4"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -2123,7 +2911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -2131,7 +2919,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -2139,13 +2927,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B12" s="4"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>37</v>
       </c>
@@ -2153,7 +2941,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -2161,7 +2949,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -2169,7 +2957,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -2279,11 +3067,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66E18A51-5F60-4412-BADD-DCCB6661D68E}">
-  <dimension ref="A1:K28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8506BFC6-2162-402B-B5AC-20BCE338FF35}">
+  <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2292,22 +3080,23 @@
     <col min="4" max="4" width="16.42578125" customWidth="1"/>
     <col min="5" max="5" width="16.5703125" customWidth="1"/>
     <col min="6" max="6" width="21.42578125" customWidth="1"/>
-    <col min="7" max="7" width="21" customWidth="1"/>
-    <col min="8" max="8" width="22.7109375" customWidth="1"/>
-    <col min="9" max="9" width="18.85546875" customWidth="1"/>
-    <col min="10" max="10" width="15.85546875" customWidth="1"/>
-    <col min="11" max="11" width="20.5703125" customWidth="1"/>
+    <col min="7" max="8" width="21" customWidth="1"/>
+    <col min="9" max="9" width="22.7109375" customWidth="1"/>
+    <col min="10" max="10" width="18.85546875" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" customWidth="1"/>
+    <col min="12" max="12" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G2" s="6"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H2" s="6"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -2319,19 +3108,22 @@
         <v>23</v>
       </c>
       <c r="H3" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="K3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="L3" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -2342,32 +3134,39 @@
         <v>40</v>
       </c>
       <c r="E4" s="6">
-        <f>Comparison!C8</f>
+        <f>Comparison!C14</f>
         <v>10000</v>
       </c>
       <c r="F4" s="7">
         <f>E4*(F5/10000)</f>
-        <v>11320.79</v>
+        <v>23386.57</v>
       </c>
       <c r="G4" s="9">
         <f>F4/E4</f>
-        <v>1.1320790000000001</v>
-      </c>
-      <c r="H4" s="7">
-        <f>E4*(H5/10000)</f>
-        <v>2181.52</v>
-      </c>
-      <c r="I4" s="9">
-        <v>0.1043</v>
+        <v>2.338657</v>
+      </c>
+      <c r="H4" s="12">
+        <f>H5</f>
+        <v>1.2</v>
+      </c>
+      <c r="I4" s="7">
+        <f>E4*(I5/10000)</f>
+        <v>6243.47</v>
       </c>
       <c r="J4" s="9">
-        <v>0.61760000000000004</v>
-      </c>
-      <c r="K4" s="8">
-        <v>918</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+        <f>J5</f>
+        <v>0.17249999999999999</v>
+      </c>
+      <c r="K4" s="9">
+        <f>K5</f>
+        <v>0.435</v>
+      </c>
+      <c r="L4" s="8">
+        <f>L5</f>
+        <v>1747</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -2378,27 +3177,29 @@
         <v>10000</v>
       </c>
       <c r="F5" s="6">
-        <v>11320.79</v>
+        <v>23386.57</v>
       </c>
       <c r="G5" s="9">
         <f>F5/E5</f>
-        <v>1.1320790000000001</v>
-      </c>
-      <c r="H5" s="6">
-        <f>2181.52</f>
-        <v>2181.52</v>
-      </c>
-      <c r="I5" s="9">
-        <v>0.1043</v>
+        <v>2.338657</v>
+      </c>
+      <c r="H5" s="12">
+        <v>1.2</v>
+      </c>
+      <c r="I5" s="6">
+        <v>6243.47</v>
       </c>
       <c r="J5" s="9">
-        <v>0.61760000000000004</v>
-      </c>
-      <c r="K5" s="8">
-        <v>918</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+        <v>0.17249999999999999</v>
+      </c>
+      <c r="K5" s="9">
+        <v>0.435</v>
+      </c>
+      <c r="L5" s="8">
+        <v>1747</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -2406,21 +3207,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="4"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -2428,7 +3229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -2436,29 +3237,29 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B12" s="4"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>37</v>
       </c>
       <c r="B13" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -2466,7 +3267,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -2474,7 +3275,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -2550,6 +3351,960 @@
       </c>
       <c r="B25">
         <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6782CC76-D1C3-4963-AF90-AA17344F07D5}">
+  <dimension ref="A1:L28"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:H1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.28515625" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" customWidth="1"/>
+    <col min="7" max="8" width="21" customWidth="1"/>
+    <col min="9" max="9" width="22.7109375" customWidth="1"/>
+    <col min="10" max="10" width="18.85546875" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" customWidth="1"/>
+    <col min="12" max="12" width="20.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="F3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>0.1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="6">
+        <f>Comparison!C14</f>
+        <v>10000</v>
+      </c>
+      <c r="F4" s="7">
+        <f>E4*(F5/10000)</f>
+        <v>14904.36</v>
+      </c>
+      <c r="G4" s="9">
+        <f>F4/E4</f>
+        <v>1.4904360000000001</v>
+      </c>
+      <c r="H4" s="12">
+        <f>H5</f>
+        <v>1.21</v>
+      </c>
+      <c r="I4" s="7">
+        <f>E4*(I5/10000)</f>
+        <v>3601.63</v>
+      </c>
+      <c r="J4" s="9">
+        <f>J5</f>
+        <v>0.13289999999999999</v>
+      </c>
+      <c r="K4" s="9">
+        <f>K5</f>
+        <v>0.36</v>
+      </c>
+      <c r="L4" s="8">
+        <f>L5</f>
+        <v>1747</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>0.5</v>
+      </c>
+      <c r="E5" s="6">
+        <v>10000</v>
+      </c>
+      <c r="F5" s="6">
+        <v>14904.36</v>
+      </c>
+      <c r="G5" s="9">
+        <f>F5/E5</f>
+        <v>1.4904360000000001</v>
+      </c>
+      <c r="H5" s="12">
+        <v>1.21</v>
+      </c>
+      <c r="I5" s="6">
+        <v>3601.63</v>
+      </c>
+      <c r="J5" s="9">
+        <v>0.13289999999999999</v>
+      </c>
+      <c r="K5" s="9">
+        <v>0.36</v>
+      </c>
+      <c r="L5" s="8">
+        <v>1747</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="4"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="4"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="5">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="4"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7F19F2C-E03C-4882-BCDB-4CC11FD1B1EA}">
+  <dimension ref="A1:L28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:H1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.28515625" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" customWidth="1"/>
+    <col min="7" max="8" width="21" customWidth="1"/>
+    <col min="9" max="9" width="22.7109375" customWidth="1"/>
+    <col min="10" max="10" width="18.85546875" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" customWidth="1"/>
+    <col min="12" max="12" width="20.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="F3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>0.1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="6">
+        <f>Comparison!C14</f>
+        <v>10000</v>
+      </c>
+      <c r="F4" s="7">
+        <f>E4*(F5/10000)</f>
+        <v>14234.069999999998</v>
+      </c>
+      <c r="G4" s="9">
+        <f>F4/E4</f>
+        <v>1.4234069999999999</v>
+      </c>
+      <c r="H4" s="12">
+        <f>H5</f>
+        <v>1.18</v>
+      </c>
+      <c r="I4" s="7">
+        <f>E4*(I5/10000)</f>
+        <v>3787.72</v>
+      </c>
+      <c r="J4" s="9">
+        <f>J5</f>
+        <v>0.14849999999999999</v>
+      </c>
+      <c r="K4" s="9">
+        <f>K5</f>
+        <v>0.42799999999999999</v>
+      </c>
+      <c r="L4" s="8">
+        <f>L5</f>
+        <v>1444</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>0.5</v>
+      </c>
+      <c r="E5" s="6">
+        <v>10000</v>
+      </c>
+      <c r="F5" s="6">
+        <v>14234.07</v>
+      </c>
+      <c r="G5" s="9">
+        <f>F5/E5</f>
+        <v>1.4234069999999999</v>
+      </c>
+      <c r="H5" s="12">
+        <v>1.18</v>
+      </c>
+      <c r="I5" s="6">
+        <v>3787.72</v>
+      </c>
+      <c r="J5" s="9">
+        <v>0.14849999999999999</v>
+      </c>
+      <c r="K5" s="9">
+        <v>0.42799999999999999</v>
+      </c>
+      <c r="L5" s="8">
+        <v>1444</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="4"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="4"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="5">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="4"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01C3B81C-4620-4EB9-8F0B-B8F5A41B29BF}">
+  <dimension ref="A1:L28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.28515625" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" customWidth="1"/>
+    <col min="7" max="8" width="21" customWidth="1"/>
+    <col min="9" max="9" width="22.7109375" customWidth="1"/>
+    <col min="10" max="10" width="18.85546875" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" customWidth="1"/>
+    <col min="12" max="12" width="20.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="F3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>0.1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="6">
+        <f>Comparison!C14</f>
+        <v>10000</v>
+      </c>
+      <c r="F4" s="7">
+        <f>E4*(F5/10000)</f>
+        <v>10926.29</v>
+      </c>
+      <c r="G4" s="9">
+        <f>F4/E4</f>
+        <v>1.0926290000000001</v>
+      </c>
+      <c r="H4" s="12">
+        <f>H5</f>
+        <v>1.21</v>
+      </c>
+      <c r="I4" s="7">
+        <f>E4*(I5/10000)</f>
+        <v>2566.5300000000002</v>
+      </c>
+      <c r="J4" s="9">
+        <f>J5</f>
+        <v>0.1178</v>
+      </c>
+      <c r="K4" s="9">
+        <f>K5</f>
+        <v>0.3518</v>
+      </c>
+      <c r="L4" s="8">
+        <f>L5</f>
+        <v>1444</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>0.5</v>
+      </c>
+      <c r="E5" s="6">
+        <v>10000</v>
+      </c>
+      <c r="F5" s="6">
+        <v>10926.29</v>
+      </c>
+      <c r="G5" s="9">
+        <f>F5/E5</f>
+        <v>1.0926290000000001</v>
+      </c>
+      <c r="H5" s="12">
+        <v>1.21</v>
+      </c>
+      <c r="I5" s="6">
+        <v>2566.5300000000002</v>
+      </c>
+      <c r="J5" s="9">
+        <v>0.1178</v>
+      </c>
+      <c r="K5" s="9">
+        <v>0.3518</v>
+      </c>
+      <c r="L5" s="8">
+        <v>1444</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="4"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="4"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="5">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="4"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25">
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>